<commit_message>
feat: read data from excel to list
</commit_message>
<xml_diff>
--- a/Assets/ExcelTest/data.xlsx
+++ b/Assets/ExcelTest/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TRI-Data\project\unity\Honda_02_2025\Assets\ExcelTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36C1B23-7535-411E-B511-002618E0BBD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C80DB2-B651-4D90-B3E8-77B99DBD681E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E1D7592F-40A0-4365-BC18-35832E9919CD}"/>
+    <workbookView xWindow="-26730" yWindow="1770" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{E1D7592F-40A0-4365-BC18-35832E9919CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Employee" sheetId="1" r:id="rId1"/>
@@ -461,7 +461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2977408B-14FB-4247-8CD9-9FB13EC02B86}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -569,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F389C9-43FF-47AA-9628-E7DCCB36479A}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,6 +639,9 @@
       <c r="C5">
         <v>10</v>
       </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>